<commit_message>
better measure of gov risk
</commit_message>
<xml_diff>
--- a/outputs_report/Table_RiskGov_ERC_tax_risk.xlsx
+++ b/outputs_report/Table_RiskGov_ERC_tax_risk.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ERC_tax_high2" r:id="rId3" sheetId="1"/>
-    <sheet name="ERC_tax_high15" r:id="rId4" sheetId="2"/>
+    <sheet name="ERC_tax_high1" r:id="rId3" sheetId="1"/>
+    <sheet name="ERC_tax_high2" r:id="rId4" sheetId="2"/>
     <sheet name="ERC_tax_hike" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
@@ -25,6 +25,60 @@
     <t>Amort</t>
   </si>
   <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>ERC_tax_PITState_a1_high1</t>
+  </si>
+  <si>
+    <t>ERC_tax_salesState_a1_high1</t>
+  </si>
+  <si>
+    <t>ERC_tax_local_a1_high1</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>port70_30</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>Discount rate = 7.5%</t>
+  </si>
+  <si>
+    <t>Discount rate = 6.0%</t>
+  </si>
+  <si>
+    <t>Fast repayment of UAAL</t>
+  </si>
+  <si>
+    <t>Slow repayment of UAAL</t>
+  </si>
+  <si>
     <t>ERC_tax_PITState_a1_high2</t>
   </si>
   <si>
@@ -32,60 +86,6 @@
   </si>
   <si>
     <t>ERC_tax_local_a1_high2</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>port70_30</t>
-  </si>
-  <si>
-    <t>normal</t>
-  </si>
-  <si>
-    <t>Discount rate = 7.5%</t>
-  </si>
-  <si>
-    <t>Discount rate = 6.0%</t>
-  </si>
-  <si>
-    <t>Fast repayment of UAAL</t>
-  </si>
-  <si>
-    <t>Slow repayment of UAAL</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>ERC_tax_PITState_a1_high15</t>
-  </si>
-  <si>
-    <t>ERC_tax_salesState_a1_high15</t>
-  </si>
-  <si>
-    <t>ERC_tax_local_a1_high15</t>
   </si>
   <si>
     <t>ERC_tax_PITState_a1_hike</t>
@@ -165,188 +165,215 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2045</v>
+        <v>30.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.143</v>
+        <v>0.33</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0815</v>
+        <v>0.2865</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.2505</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.1585</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.078</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>0.0095</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0195</v>
+        <v>30.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0035</v>
+        <v>0.168</v>
       </c>
       <c r="G4" t="n">
-        <v>0.001</v>
+        <v>0.0975</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0475</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01</v>
+        <v>30.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0</v>
+        <v>0.06</v>
       </c>
       <c r="G5" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1005</v>
+        <v>30.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0835</v>
+        <v>0.2455</v>
       </c>
       <c r="G6" t="n">
-        <v>0.07</v>
+        <v>0.2465</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.242</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="F7" t="n">
         <v>0.0525</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>0.0275</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>0.002</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" t="n">
-        <v>0.001</v>
+        <v>30.0</v>
       </c>
       <c r="F8" t="n">
-        <v>5.0E-4</v>
+        <v>0.057</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0</v>
+        <v>0.044</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.035</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0105</v>
+      </c>
+      <c r="G9" t="n">
         <v>5.0E-4</v>
       </c>
-      <c r="F9" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -375,223 +402,196 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" t="n">
-        <v>30.0</v>
+        <v>0.3485</v>
       </c>
       <c r="F2" t="n">
-        <v>0.45</v>
+        <v>0.302</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4045</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.3945</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="n">
-        <v>30.0</v>
+        <v>0.0665</v>
       </c>
       <c r="F3" t="n">
-        <v>0.396</v>
+        <v>0.012</v>
       </c>
       <c r="G3" t="n">
-        <v>0.345</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.3195</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n">
-        <v>30.0</v>
+        <v>1.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1195</v>
+        <v>1.0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.0225</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
-        <v>30.0</v>
+        <v>0.1135</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0785</v>
+        <v>0.0345</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0175</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.0</v>
+        <v>0.0015</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" t="n">
-        <v>30.0</v>
+        <v>0.2655</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3905</v>
+        <v>0.2705</v>
       </c>
       <c r="G6" t="n">
-        <v>0.415</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.408</v>
+        <v>0.2695</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
-        <v>30.0</v>
+        <v>0.009</v>
       </c>
       <c r="F7" t="n">
-        <v>0.308</v>
+        <v>5.0E-4</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3015</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.2905</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" t="n">
-        <v>30.0</v>
+        <v>1.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.035</v>
+        <v>1.0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0205</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.01</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" t="n">
-        <v>30.0</v>
+        <v>0.035</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0195</v>
+        <v>0.0085</v>
       </c>
       <c r="G9" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="H9" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -620,7 +620,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>24</v>
@@ -634,16 +634,16 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2" t="n">
         <v>30.0</v>
@@ -660,16 +660,16 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="n">
         <v>30.0</v>
@@ -686,16 +686,16 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="n">
         <v>30.0</v>
@@ -712,16 +712,16 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
         <v>30.0</v>
@@ -738,42 +738,42 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" t="n">
         <v>30.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3815</v>
+        <v>0.3795</v>
       </c>
       <c r="G6" t="n">
-        <v>0.363</v>
+        <v>0.3675</v>
       </c>
       <c r="H6" t="n">
-        <v>0.339</v>
+        <v>0.352</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
         <v>30.0</v>
@@ -790,42 +790,42 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" t="n">
         <v>30.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.351</v>
+        <v>0.3365</v>
       </c>
       <c r="G8" t="n">
-        <v>0.334</v>
+        <v>0.326</v>
       </c>
       <c r="H8" t="n">
-        <v>0.3205</v>
+        <v>0.315</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E9" t="n">
         <v>30.0</v>

</xml_diff>